<commit_message>
cambios del seguimiento de pila
</commit_message>
<xml_diff>
--- a/SeguimientoEjercicioPila.xlsx
+++ b/SeguimientoEjercicioPila.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Desktop\Universidad\2020-1\ArquiHard\lab\ArquitecturaHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D810F1B-81C8-4AF1-B7FC-605CF9CBB0DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BEFEF6-EA64-47EC-ACE1-42567A8EB43B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{829AEDDF-D318-4274-845D-855B172866FF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t xml:space="preserve">Dirección </t>
   </si>
@@ -84,24 +84,6 @@
     <t>0019FE40</t>
   </si>
   <si>
-    <t>0x770d6359</t>
-  </si>
-  <si>
-    <t>[ecx-4]</t>
-  </si>
-  <si>
-    <t>ebp</t>
-  </si>
-  <si>
-    <t>ecx</t>
-  </si>
-  <si>
-    <t>(esp original)</t>
-  </si>
-  <si>
-    <t>(esp estuvo aquí)</t>
-  </si>
-  <si>
     <t xml:space="preserve">0019ff4c </t>
   </si>
   <si>
@@ -145,6 +127,84 @@
   </si>
   <si>
     <t>Ret main</t>
+  </si>
+  <si>
+    <t>0) esp 0x19ff74</t>
+  </si>
+  <si>
+    <t>ECX=0019FF78</t>
+  </si>
+  <si>
+    <t>1)esp 0x19ff70</t>
+  </si>
+  <si>
+    <t>lea     ecx, [esp+4]</t>
+  </si>
+  <si>
+    <t>2) esp 0x19ff6c</t>
+  </si>
+  <si>
+    <t>push    DWORD PTR [ecx-4]</t>
+  </si>
+  <si>
+    <t>3)esp 0x19ff68</t>
+  </si>
+  <si>
+    <t>4) esp 0x19ff64</t>
+  </si>
+  <si>
+    <t>5) sub esp, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6) sub esp, 12 </t>
+  </si>
+  <si>
+    <t>esp 0x19ff54</t>
+  </si>
+  <si>
+    <t>7) 0x19ff50</t>
+  </si>
+  <si>
+    <t>8) esp 0x19ff4c</t>
+  </si>
+  <si>
+    <t>9) esp 0x19ff68</t>
+  </si>
+  <si>
+    <t>mov ebp, esp</t>
+  </si>
+  <si>
+    <t>ret main</t>
+  </si>
+  <si>
+    <t>push ebp</t>
+  </si>
+  <si>
+    <t>push ecx</t>
+  </si>
+  <si>
+    <t>10)  pop     ebp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11)"pop" de ret </t>
+  </si>
+  <si>
+    <t>11)  add     esp, 16</t>
+  </si>
+  <si>
+    <t>12) mov  esp,ebp</t>
+  </si>
+  <si>
+    <t>13) pop     ebp</t>
+  </si>
+  <si>
+    <t>14) lea     esp, [ecx-4]</t>
+  </si>
+  <si>
+    <t>Parametro de la función</t>
+  </si>
+  <si>
+    <t>Salida de la función</t>
   </si>
 </sst>
 </file>
@@ -214,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -274,11 +334,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,18 +362,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,16 +398,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1461969</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>185173</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>185059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>763839</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>115</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5255</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -354,7 +430,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3073892" y="1753135"/>
+          <a:off x="8132885" y="1950847"/>
           <a:ext cx="767255" cy="210595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -362,6 +438,235 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21980</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1150327</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C310BA74-EFA0-43BD-972E-EC9918AE946F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4769826" y="4931019"/>
+          <a:ext cx="1128347" cy="197827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO"/>
+            <a:t>←</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>  EBP</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CuadroTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFE29A46-3D40-423C-A069-26CCF2704502}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3253155" y="5524501"/>
+          <a:ext cx="1494692" cy="989134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>Se agregar la variable A al registro EAX y  se hace un push de EAX</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0"/>
+            <a:t> para pasarle el valor de A a  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>FuncInc_int</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>197826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE0C465E-12C6-4D14-909F-C7D1C0F34384}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3253154" y="6909288"/>
+          <a:ext cx="1494692" cy="1538654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0"/>
+            <a:t>El resultado de la función se suma en el registro eax, cuando se hace el ret regresa a la siguiente instrucción del call. Donde a la variable local A se remplaza por eax.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -664,239 +969,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683F196D-63A5-475C-A6AF-AD808C16853A}">
-  <dimension ref="A3:D37"/>
+  <dimension ref="A3:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="10"/>
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="11"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="12"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>26</v>
+      <c r="C22" s="12"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
   </sheetData>

</xml_diff>